<commit_message>
added dates to axis from team request
</commit_message>
<xml_diff>
--- a/deliverables/ganttChartAvocadoBudget.xlsx
+++ b/deliverables/ganttChartAvocadoBudget.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcronauer/Desktop/ceg4110-group-project-avocadobudget/deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398D2E75-0FE2-7A41-9FC0-DFA295DD1F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6C69D3-FC5B-5145-A5CD-1EE40B9EEAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AB48C4DA-0DA3-C24A-B5FB-8C34E6C351BB}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{AB48C4DA-0DA3-C24A-B5FB-8C34E6C351BB}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChartGraph" sheetId="2" r:id="rId1"/>
     <sheet name="ganttByWeek" sheetId="5" r:id="rId2"/>
-    <sheet name="ganttChart" sheetId="1" r:id="rId3"/>
-    <sheet name="ganttChartDays" sheetId="3" r:id="rId4"/>
-    <sheet name="graphDays" sheetId="4" r:id="rId5"/>
+    <sheet name="ganttChartDaysGraph" sheetId="6" r:id="rId3"/>
+    <sheet name="ganttChart" sheetId="1" r:id="rId4"/>
+    <sheet name="ganttChartDays" sheetId="3" r:id="rId5"/>
+    <sheet name="graphDays" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -213,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -233,6 +234,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1862,6 +1864,478 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ganttChartDays!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ganttChartDays!$E$2:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Team Composition Form</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Project Overview Proposal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Software Development Plan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>User Story Compendium</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MVS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Requirements Specification</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Wireframe</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Table Design</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Design Specificaition</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>CRUD operations</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>UI Tasks Complete</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Business Logic / Code complete</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>HTML / CSS - Finailzed</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Reports - integrate for reports</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Additional Features as time allows</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Testing / Finalizing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ganttChartDays!$F$2:$F$30</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>45531</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45534</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45541</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45548</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45555</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45557</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45557</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45551</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45562</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45565</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45564</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45579</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45579</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45593</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45607</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4E0B-224B-8DE5-156B71638E7D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Duration</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ganttChartDays!$E$2:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Team Composition Form</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Project Overview Proposal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Software Development Plan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>User Story Compendium</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MVS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Requirements Specification</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Wireframe</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Table Design</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Design Specificaition</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>CRUD operations</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>UI Tasks Complete</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Business Logic / Code complete</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>HTML / CSS - Finailzed</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Reports - integrate for reports</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Additional Features as time allows</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Testing / Finalizing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ganttChartDays!$H$2:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4E0B-224B-8DE5-156B71638E7D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="113319872"/>
+        <c:axId val="363256416"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="113319872"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="363256416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="363256416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="45634"/>
+          <c:min val="45531"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="113319872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2530,6 +3004,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -4046,6 +4560,511 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4673,6 +5692,47 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B3913A0-6D64-D238-C21B-E7E8D0118792}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5046,21 +6106,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA06594-E37E-024F-9826-B8894DB230AE}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="88" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0B58A8-1725-9346-8D7A-A2B2A8A679BC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDBD315-BC6F-C442-A28D-8A53B67687F2}">
   <dimension ref="A1:T103"/>
   <sheetViews>
@@ -6780,12 +7858,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206F12A4-D5C5-3344-A090-044D9A9789D4}">
   <dimension ref="A1:X103"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6868,12 +7946,12 @@
         <v>45531</v>
       </c>
       <c r="G2" s="8">
-        <f>VLOOKUP(D2,$I:$K,3,FALSE)</f>
+        <f t="shared" ref="G2:G17" si="0">VLOOKUP(D2,$I:$K,3,FALSE)</f>
         <v>45534</v>
       </c>
-      <c r="H2" s="8">
-        <f t="shared" ref="H2" si="0">VLOOKUP(C2,$I:$K,3,FALSE)</f>
-        <v>45533</v>
+      <c r="H2" s="9">
+        <f>C2</f>
+        <v>3</v>
       </c>
       <c r="I2" s="5">
         <v>2</v>
@@ -6917,12 +7995,12 @@
         <v>45534</v>
       </c>
       <c r="G3" s="8">
-        <f>VLOOKUP(D3,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45541</v>
       </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H17" si="3">VLOOKUP(C3,$I:$K,3,FALSE)</f>
-        <v>45537</v>
+      <c r="H3" s="9">
+        <f t="shared" ref="H3:H17" si="3">C3</f>
+        <v>7</v>
       </c>
       <c r="I3" s="5">
         <v>3</v>
@@ -6965,12 +8043,12 @@
         <v>45541</v>
       </c>
       <c r="G4" s="8">
-        <f>VLOOKUP(D4,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45548</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="9">
         <f t="shared" si="3"/>
-        <v>45537</v>
+        <v>7</v>
       </c>
       <c r="I4" s="5">
         <v>4</v>
@@ -7013,12 +8091,12 @@
         <v>45548</v>
       </c>
       <c r="G5" s="8">
-        <f>VLOOKUP(D5,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45555</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="9">
         <f t="shared" si="3"/>
-        <v>45537</v>
+        <v>7</v>
       </c>
       <c r="I5" s="5">
         <v>5</v>
@@ -7061,12 +8139,12 @@
         <v>45555</v>
       </c>
       <c r="G6" s="8">
-        <f>VLOOKUP(D6,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45557</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="9">
         <f t="shared" si="3"/>
-        <v>45532</v>
+        <v>2</v>
       </c>
       <c r="I6" s="5">
         <v>6</v>
@@ -7103,12 +8181,12 @@
         <v>45557</v>
       </c>
       <c r="G7" s="8">
-        <f>VLOOKUP(D7,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45562</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="9">
         <f t="shared" si="3"/>
-        <v>45535</v>
+        <v>5</v>
       </c>
       <c r="I7" s="5">
         <v>7</v>
@@ -7151,12 +8229,12 @@
         <v>45557</v>
       </c>
       <c r="G8" s="8">
-        <f>VLOOKUP(D8,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45564</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="9">
         <f t="shared" si="3"/>
-        <v>45537</v>
+        <v>7</v>
       </c>
       <c r="I8" s="5">
         <v>8</v>
@@ -7199,12 +8277,12 @@
         <v>45551</v>
       </c>
       <c r="G9" s="8">
-        <f>VLOOKUP(D9,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45565</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="9">
         <f t="shared" si="3"/>
-        <v>45544</v>
+        <v>14</v>
       </c>
       <c r="I9" s="5">
         <v>9</v>
@@ -7247,12 +8325,12 @@
         <v>45562</v>
       </c>
       <c r="G10" s="8">
-        <f>VLOOKUP(D10,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45576</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="9">
         <f t="shared" si="3"/>
-        <v>45544</v>
+        <v>14</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
@@ -7295,12 +8373,12 @@
         <v>45565</v>
       </c>
       <c r="G11" s="8">
-        <f>VLOOKUP(D11,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45579</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="9">
         <f t="shared" si="3"/>
-        <v>45544</v>
+        <v>14</v>
       </c>
       <c r="I11" s="5">
         <v>11</v>
@@ -7343,12 +8421,12 @@
         <v>45564</v>
       </c>
       <c r="G12" s="8">
-        <f>VLOOKUP(D12,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45578</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="9">
         <f t="shared" si="3"/>
-        <v>45544</v>
+        <v>14</v>
       </c>
       <c r="I12" s="5">
         <v>12</v>
@@ -7385,12 +8463,12 @@
         <v>45579</v>
       </c>
       <c r="G13" s="8">
-        <f>VLOOKUP(D13,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45593</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="9">
         <f t="shared" si="3"/>
-        <v>45544</v>
+        <v>14</v>
       </c>
       <c r="I13" s="5">
         <v>13</v>
@@ -7424,12 +8502,12 @@
         <v>45579</v>
       </c>
       <c r="G14" s="8">
-        <f>VLOOKUP(D14,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45593</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="9">
         <f t="shared" si="3"/>
-        <v>45544</v>
+        <v>14</v>
       </c>
       <c r="I14" s="5">
         <v>14</v>
@@ -7463,12 +8541,12 @@
         <v>45593</v>
       </c>
       <c r="G15" s="8">
-        <f>VLOOKUP(D15,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45600</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="9">
         <f t="shared" si="3"/>
-        <v>45537</v>
+        <v>7</v>
       </c>
       <c r="I15" s="5">
         <v>15</v>
@@ -7502,12 +8580,12 @@
         <v>45600</v>
       </c>
       <c r="G16" s="8">
-        <f>VLOOKUP(D16,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45607</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="9">
         <f t="shared" si="3"/>
-        <v>45537</v>
+        <v>7</v>
       </c>
       <c r="I16" s="5">
         <v>16</v>
@@ -7541,12 +8619,12 @@
         <v>45607</v>
       </c>
       <c r="G17" s="8">
-        <f>VLOOKUP(D17,$I:$K,3,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>45621</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="9">
         <f t="shared" si="3"/>
-        <v>45544</v>
+        <v>14</v>
       </c>
       <c r="I17" s="5">
         <v>17</v>
@@ -8596,7 +9674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BEB16E8-A4A7-1D4C-900E-6ED99D8AC7D1}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
changed excel file chart, new pdf, removed old pdf, so gantt chart displays by data rather than week
</commit_message>
<xml_diff>
--- a/deliverables/ganttChartAvocadoBudget.xlsx
+++ b/deliverables/ganttChartAvocadoBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcronauer/Desktop/ceg4110-group-project-avocadobudget/deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6C69D3-FC5B-5145-A5CD-1EE40B9EEAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8519A541-2A57-D646-8017-E3C2930373AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{AB48C4DA-0DA3-C24A-B5FB-8C34E6C351BB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{AB48C4DA-0DA3-C24A-B5FB-8C34E6C351BB}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChartGraph" sheetId="2" r:id="rId1"/>
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,6 +235,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1877,9 +1878,87 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Gantt</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart Avocado Budget</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40295128939828079"/>
+          <c:y val="1.9108280254777069E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20833032511337232"/>
+          <c:y val="0.22686293194242441"/>
+          <c:w val="0.76337014642510659"/>
+          <c:h val="0.73525912013291916"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
@@ -2228,7 +2307,7 @@
         <c:axId val="363256416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45634"/>
+          <c:max val="45626"/>
           <c:min val="45531"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2259,7 +2338,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2281,7 +2360,8 @@
         <c:crossAx val="113319872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="7"/>
+        <c:minorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5696,15 +5776,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6125,15 +6205,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0B58A8-1725-9346-8D7A-A2B2A8A679BC}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="15" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N15" s="10"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>